<commit_message>
update for manuscript revision
added new studies, updated plots and added folder for effort preferences
</commit_message>
<xml_diff>
--- a/data/study_data_codebook.xlsx
+++ b/data/study_data_codebook.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abagaini/Documents/PROJECTS/Cumul_MA/cumulative/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D574F65-5DB1-6E48-9D2E-06595550A94D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E35738-1E0E-5B48-8747-DA864E632578}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="20660" xr2:uid="{A9CBDFF5-18E2-AE44-855C-359BC31DE105}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17060" xr2:uid="{A9CBDFF5-18E2-AE44-855C-359BC31DE105}"/>
   </bookViews>
   <sheets>
     <sheet name="codebook" sheetId="1" r:id="rId1"/>
+    <sheet name="codebook_effort" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">codebook!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">codebook_effort!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="146">
   <si>
     <t>first_author</t>
   </si>
@@ -455,12 +457,24 @@
   <si>
     <t>From where was the outcome information obtained: directly from article, figure or raw data</t>
   </si>
+  <si>
+    <t>effort_type</t>
+  </si>
+  <si>
+    <t>Type of effort that participants need to exert: Physical or Cognitive</t>
+  </si>
+  <si>
+    <t>study_context</t>
+  </si>
+  <si>
+    <t>Was the study coducted in-person (e.g., lab) or online</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -477,10 +491,15 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -503,7 +522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -516,6 +535,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -834,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C0E0E3-3547-5447-BF12-845DBFB44825}">
   <dimension ref="A1:E16385"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="186" zoomScaleNormal="186" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -847,1035 +876,1035 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="8" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E2"/>
     </row>
     <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>131</v>
       </c>
       <c r="E3"/>
     </row>
     <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E4"/>
     </row>
     <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="8" t="s">
         <v>131</v>
       </c>
       <c r="E5"/>
     </row>
     <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E6"/>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="8" t="s">
         <v>131</v>
       </c>
       <c r="E7"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="8" t="s">
         <v>131</v>
       </c>
       <c r="E8"/>
     </row>
     <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="8" t="s">
         <v>131</v>
       </c>
       <c r="E9"/>
     </row>
     <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="8" t="s">
         <v>131</v>
       </c>
       <c r="E10"/>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="8" t="s">
         <v>131</v>
       </c>
       <c r="E11"/>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="8" t="s">
         <v>131</v>
       </c>
       <c r="E12"/>
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E13"/>
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E14"/>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E15"/>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E16"/>
     </row>
     <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E17"/>
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+      <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E18"/>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
+      <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E19"/>
     </row>
     <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
+      <c r="A20" s="5">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E20"/>
     </row>
     <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
+      <c r="A21" s="5">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E21"/>
     </row>
     <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
+      <c r="A22" s="5">
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E22"/>
     </row>
     <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
+      <c r="A23" s="5">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E23"/>
     </row>
     <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
+      <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E24"/>
     </row>
     <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
+      <c r="A25" s="5">
         <v>24</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E25"/>
     </row>
     <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
+      <c r="A26" s="5">
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E26"/>
     </row>
     <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
+      <c r="A27" s="5">
         <v>26</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E27"/>
     </row>
     <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
+      <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E28"/>
     </row>
     <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
+      <c r="A29" s="5">
         <v>28</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E29"/>
     </row>
     <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
+      <c r="A30" s="5">
         <v>29</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E30"/>
     </row>
     <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
+      <c r="A31" s="5">
         <v>30</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E31"/>
     </row>
     <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
+      <c r="A32" s="5">
         <v>31</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E32"/>
     </row>
     <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
+      <c r="A33" s="5">
         <v>32</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E33"/>
     </row>
     <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
+      <c r="A34" s="5">
         <v>33</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E34"/>
     </row>
     <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
+      <c r="A35" s="5">
         <v>34</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E35"/>
     </row>
     <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
+      <c r="A36" s="5">
         <v>35</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E36"/>
     </row>
     <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
+      <c r="A37" s="5">
         <v>36</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E37"/>
     </row>
     <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
+      <c r="A38" s="5">
         <v>37</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E38"/>
     </row>
     <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
+      <c r="A39" s="5">
         <v>38</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E39"/>
     </row>
     <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
+      <c r="A40" s="5">
         <v>39</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E40"/>
     </row>
     <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
+      <c r="A41" s="5">
         <v>40</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E41"/>
     </row>
     <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="1">
+      <c r="A42" s="5">
         <v>41</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E42"/>
     </row>
     <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="1">
+      <c r="A43" s="5">
         <v>42</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E43"/>
     </row>
     <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="1">
+      <c r="A44" s="5">
         <v>43</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E44"/>
     </row>
     <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="1">
+      <c r="A45" s="5">
         <v>44</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E45"/>
     </row>
     <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="1">
+      <c r="A46" s="5">
         <v>45</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E46"/>
     </row>
     <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="1">
+      <c r="A47" s="5">
         <v>46</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E47"/>
     </row>
     <row r="48" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="1">
+      <c r="A48" s="5">
         <v>47</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E48"/>
     </row>
     <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="1">
+      <c r="A49" s="5">
         <v>48</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E49"/>
     </row>
     <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="1">
+      <c r="A50" s="5">
         <v>49</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E50"/>
     </row>
     <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" s="1">
+      <c r="A51" s="5">
         <v>50</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E51"/>
     </row>
     <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="1">
+      <c r="A52" s="5">
         <v>51</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E52"/>
     </row>
     <row r="53" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="1">
+      <c r="A53" s="5">
         <v>52</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D53" s="8" t="s">
         <v>131</v>
       </c>
       <c r="E53"/>
     </row>
     <row r="54" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="1">
+      <c r="A54" s="5">
         <v>53</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" s="8" t="s">
         <v>131</v>
       </c>
       <c r="E54"/>
     </row>
     <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A55" s="1">
+      <c r="A55" s="5">
         <v>54</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E55"/>
     </row>
     <row r="56" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="1">
+      <c r="A56" s="5">
         <v>55</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="D56" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E56"/>
     </row>
     <row r="57" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A57" s="1">
+      <c r="A57" s="5">
         <v>56</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D57" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E57"/>
     </row>
     <row r="58" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" s="1">
+      <c r="A58" s="5">
         <v>57</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D58" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E58"/>
     </row>
     <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="1">
+      <c r="A59" s="5">
         <v>58</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E59"/>
     </row>
     <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A60" s="1">
+      <c r="A60" s="5">
         <v>59</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="D60" s="4" t="s">
+      <c r="D60" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E60"/>
     </row>
     <row r="61" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" s="1">
+      <c r="A61" s="5">
         <v>60</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D61" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E61"/>
     </row>
     <row r="62" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" s="1">
+      <c r="A62" s="5">
         <v>61</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D62" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E62"/>
     </row>
     <row r="63" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="1">
+      <c r="A63" s="5">
         <v>62</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="D63" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E63"/>
     </row>
     <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="1">
+      <c r="A64" s="5">
         <v>63</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="D64" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E64"/>
     </row>
     <row r="65" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A65" s="1">
+      <c r="A65" s="5">
         <v>64</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D65" s="8" t="s">
         <v>131</v>
       </c>
       <c r="E65"/>
     </row>
     <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A66" s="1">
+      <c r="A66" s="5">
         <v>65</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B66" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C66" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D66" s="8" t="s">
         <v>131</v>
       </c>
       <c r="E66"/>
     </row>
     <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A67" s="1">
+      <c r="A67" s="5">
         <v>66</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B67" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C67" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D67" s="8" t="s">
         <v>131</v>
       </c>
       <c r="E67"/>
     </row>
     <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A68" s="1">
+      <c r="A68" s="5">
         <v>67</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B68" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C68" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D68" s="8" t="s">
         <v>131</v>
       </c>
       <c r="E68"/>
     </row>
     <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A69" s="1">
+      <c r="A69" s="5">
         <v>68</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C69" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="D69" s="8" t="s">
         <v>131</v>
       </c>
       <c r="E69"/>
@@ -50827,6 +50856,1021 @@
     </row>
     <row r="16385" spans="5:5" ht="16" x14ac:dyDescent="0.2">
       <c r="E16385"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0023B6-9A7A-2643-BFDB-206E4D988043}">
+  <dimension ref="A1:D71"/>
+  <sheetViews>
+    <sheetView topLeftCell="A58" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="26" style="6" customWidth="1"/>
+    <col min="3" max="3" width="51.1640625" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
+        <v>32</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
+        <v>33</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
+        <v>34</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
+        <v>35</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A37" s="5">
+        <v>36</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
+        <v>37</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A39" s="5">
+        <v>38</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A40" s="5">
+        <v>39</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A41" s="5">
+        <v>40</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A42" s="5">
+        <v>41</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A43" s="5">
+        <v>42</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A44" s="5">
+        <v>43</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A45" s="5">
+        <v>44</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A46" s="5">
+        <v>45</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A47" s="5">
+        <v>46</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A48" s="5">
+        <v>47</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A49" s="5">
+        <v>48</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A50" s="5">
+        <v>49</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A51" s="5">
+        <v>50</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A52" s="5">
+        <v>51</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A53" s="5">
+        <v>52</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A54" s="5">
+        <v>53</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A55" s="5">
+        <v>54</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A56" s="5">
+        <v>55</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A57" s="5">
+        <v>56</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A58" s="5">
+        <v>57</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A59" s="5">
+        <v>58</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A60" s="5">
+        <v>59</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A61" s="5">
+        <v>60</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A62" s="5">
+        <v>61</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A63" s="5">
+        <v>62</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A64" s="5">
+        <v>63</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A65" s="5">
+        <v>64</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A66" s="5">
+        <v>65</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A67" s="5">
+        <v>66</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A68" s="5">
+        <v>67</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A69" s="5">
+        <v>68</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A70" s="5">
+        <v>69</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A71" s="5">
+        <v>70</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>131</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>